<commit_message>
working on lr-crf understander
</commit_message>
<xml_diff>
--- a/sample_apps/simple_ja/simple-nlu-knowledge-ja.xlsx
+++ b/sample_apps/simple_ja/simple-nlu-knowledge-ja.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\sample_apps\simple_ja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E8330E-1370-4893-B120-5EBF8E9C3224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B21D7F-5B20-4457-BA88-1D2B1DBA2C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="83" yWindow="1567" windowWidth="21600" windowHeight="11296" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="utterances" sheetId="2" r:id="rId1"/>
@@ -476,60 +476,34 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>富山</t>
+    <rPh sb="0" eb="2">
+      <t>トヤマ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>佐野</t>
+    <rPh sb="0" eb="2">
+      <t>サノ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>博多</t>
+    <rPh sb="0" eb="2">
+      <t>ハカタ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>肯定</t>
+  </si>
+  <si>
+    <t>地方=札幌, 好きなラーメン=味噌ラーメン</t>
+  </si>
+  <si>
     <t>地方=博多、好きなラーメン=豚骨ラーメン</t>
-    <rPh sb="0" eb="2">
-      <t>チホウ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ハカタ</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>ス</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>トンコツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>富山</t>
-    <rPh sb="0" eb="2">
-      <t>トヤマ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>佐野</t>
-    <rPh sb="0" eb="2">
-      <t>サノ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>博多</t>
-    <rPh sb="0" eb="2">
-      <t>ハカタ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>地方=札幌, 好きなラーメン=味噌ラーメン</t>
-    <rPh sb="0" eb="2">
-      <t>チホウ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>サッポロ</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>ス</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>ミソ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>肯定</t>
   </si>
 </sst>
 </file>
@@ -927,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8F96FF-CF47-4A99-83E7-8D5E860D6DFF}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -957,7 +931,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -968,7 +942,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -979,7 +953,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -1259,7 +1233,7 @@
         <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1375,7 +1349,7 @@
         <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1386,7 +1360,7 @@
         <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1397,7 +1371,7 @@
         <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>